<commit_message>
Try to fix 4COM03_Metabolomics
</commit_message>
<xml_diff>
--- a/templates/4COM03_Metabolomics/4COM03_Metabolomics.xlsx
+++ b/templates/4COM03_Metabolomics/4COM03_Metabolomics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/DataManagementPlans/SWATE_templates/templates/4COM03_Metabolomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A6302B-A8E9-534E-ABD6-72A087809934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3C02FC-5B4D-BA4C-8C57-EDA2C04FC330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4740" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
+    <workbookView xWindow="-4700" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
   <sheets>
     <sheet name="4COM03_Metabolomics" sheetId="5" r:id="rId1"/>
@@ -1144,7 +1144,7 @@
       <pane xSplit="2" ySplit="12" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="S8" sqref="S8:S9"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
shaping swate templates (4COM batch)
</commit_message>
<xml_diff>
--- a/templates/4COM03_Metabolomics/4COM03_Metabolomics.xlsx
+++ b/templates/4COM03_Metabolomics/4COM03_Metabolomics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/DataManagementPlans/SWATE_templates/templates/4COM03_Metabolomics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/MetadataTemplates/SWATE_templates/templates/4COM03_Metabolomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3C02FC-5B4D-BA4C-8C57-EDA2C04FC330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F52268D-CC14-6D43-9D9F-EC66534F0D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4700" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
@@ -24,81 +24,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Dominik Brilhaus</author>
-  </authors>
-  <commentList>
-    <comment ref="B23" authorId="0" shapeId="0" xr:uid="{140CBE1F-7B48-134E-9B41-9BC85F1D4E84}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Dominik Brilhaus:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">cv: controlled vocabulary
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">m: mandatory 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">o: optional (can be mapped)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>n: not required (cannot be mapped)</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
   <si>
     <t>Source Name</t>
   </si>
@@ -106,48 +33,18 @@
     <t>Sample Name</t>
   </si>
   <si>
-    <t>SWATE annotation table</t>
-  </si>
-  <si>
-    <t>Content examples</t>
-  </si>
-  <si>
-    <t>Semantic Modelling</t>
-  </si>
-  <si>
     <t>Term Name</t>
   </si>
   <si>
     <t>Term Accession Number (TAN)</t>
   </si>
   <si>
-    <t>URI</t>
-  </si>
-  <si>
-    <t>is_a</t>
-  </si>
-  <si>
-    <t>is_a URI</t>
-  </si>
-  <si>
     <t>Content type (Validation)</t>
   </si>
   <si>
-    <t xml:space="preserve">Comment: </t>
-  </si>
-  <si>
     <t>ER target term</t>
   </si>
   <si>
-    <t>ER requirement (cv/m/o/n)</t>
-  </si>
-  <si>
-    <t>Importance (0-5)</t>
-  </si>
-  <si>
-    <t>Justification</t>
-  </si>
-  <si>
     <t>Additional information</t>
   </si>
   <si>
@@ -221,13 +118,98 @@
   </si>
   <si>
     <t>*.mzData</t>
+  </si>
+  <si>
+    <t>SWATE_annotation_table</t>
+  </si>
+  <si>
+    <t>SWATE templating version (July 26, 2021)</t>
+  </si>
+  <si>
+    <t>content_examples</t>
+  </si>
+  <si>
+    <t>semantics_SWATE</t>
+  </si>
+  <si>
+    <t>Name of term (to be) linked in SWATE template</t>
+  </si>
+  <si>
+    <t>TAN (to be) linked in SWATE template</t>
+  </si>
+  <si>
+    <t>Term URI</t>
+  </si>
+  <si>
+    <t>URI of term (to be) linked in SWATE template</t>
+  </si>
+  <si>
+    <t>Info for SWATE checklist editor</t>
+  </si>
+  <si>
+    <t>semantics_other</t>
+  </si>
+  <si>
+    <t>Additional instruction we want to share for user convenience</t>
+  </si>
+  <si>
+    <t>Notes during templating</t>
+  </si>
+  <si>
+    <t>semantics_nfdi4pso</t>
+  </si>
+  <si>
+    <t>xref term</t>
+  </si>
+  <si>
+    <t>Use for exact matches to terms from ontologies that are not imported to or part of swateDB</t>
+  </si>
+  <si>
+    <t>xref URI</t>
+  </si>
+  <si>
+    <t>synonym</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>Name of the term in the ER target. This is what the SWATE template maps to.</t>
+  </si>
+  <si>
+    <t>ER instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User instructions coming from the ER (typcially as excel comments). May hold info for requirements of certain terms. </t>
+  </si>
+  <si>
+    <t>ER requirement (m/o/n)</t>
+  </si>
+  <si>
+    <t>m: mandatory 
+o: optional (can be mapped)
+n: not required (cannot be mapped)</t>
+  </si>
+  <si>
+    <t>ER value (cv/s/d)</t>
+  </si>
+  <si>
+    <t>cv: controlled vocabulary
+s: free string
+d: number</t>
+  </si>
+  <si>
+    <t>Anything particular we need to be aware of</t>
+  </si>
+  <si>
+    <t>Comments towards the original template author</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -266,23 +248,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -371,7 +360,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -394,22 +383,15 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -418,14 +400,53 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,8 +821,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CB2092AC-614F-704E-8871-2BD6E7F964FB}" name="annotationTable" displayName="annotationTable" ref="C2:Q3" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="C2:Q3" xr:uid="{208E1453-2FC4-AF4B-A87A-2C5775F13953}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CB2092AC-614F-704E-8871-2BD6E7F964FB}" name="annotationTable" displayName="annotationTable" ref="D2:R3" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="D2:R3" xr:uid="{208E1453-2FC4-AF4B-A87A-2C5775F13953}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{1408720F-A080-F948-9E9A-11F5844E0CF9}" name="Source Name" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{EBF6BEE7-75C2-DB4A-A875-26F210730C86}" name="Sample Name" dataDxfId="13"/>
@@ -1137,45 +1158,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBB40E6-F06B-AE48-B869-B32AACDBDD09}">
-  <dimension ref="A1:Q29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBB40E6-F06B-AE48-B869-B32AACDBDD09}">
+  <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="12" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="13" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.1640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="52.83203125" style="19" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="59" style="19" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="31.1640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="53.83203125" style="19" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="60.1640625" style="19" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="30.1640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="52.83203125" style="19" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="59" style="19" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="37.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="66.33203125" style="19" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="72.5" style="19" hidden="1" customWidth="1"/>
-    <col min="18" max="16384" width="11" style="19"/>
+    <col min="1" max="1" width="34.33203125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="42.6640625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.83203125" style="14" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="59" style="14" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="31.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="53.83203125" style="14" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="60.1640625" style="14" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="30.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="52.83203125" style="14" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="59" style="14" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="37.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="66.33203125" style="14" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="72.5" style="14" hidden="1" customWidth="1"/>
+    <col min="19" max="16384" width="11" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -1188,365 +1212,692 @@
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
-      <c r="Q1" s="2"/>
-    </row>
-    <row r="2" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q1" s="3"/>
+      <c r="R1" s="2"/>
+    </row>
+    <row r="2" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="E2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="F2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="Q2" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="R2" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="23" t="s">
+    </row>
+    <row r="3" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C3" s="4"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="33"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="33"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+    </row>
+    <row r="12" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+    </row>
+    <row r="13" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="E5" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="23" t="s">
+      <c r="C13" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+    </row>
+    <row r="14" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23" t="s">
+      <c r="B14" s="9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="E6" s="23" t="s">
+      <c r="C14" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23" t="s">
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+    </row>
+    <row r="15" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23" t="s">
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+    </row>
+    <row r="16" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="8" t="s">
+      <c r="B16" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+    </row>
+    <row r="18" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
+    </row>
+    <row r="19" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="28"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="28"/>
+      <c r="P23" s="28"/>
+    </row>
+    <row r="24" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="10" t="s">
+      <c r="C24" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="25"/>
+    </row>
+    <row r="25" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="30"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="30"/>
+      <c r="P25" s="30"/>
+    </row>
+    <row r="26" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="30"/>
+    </row>
+    <row r="27" spans="1:16" s="16" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
+    </row>
+    <row r="28" spans="1:16" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="24" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="11" t="s">
+      <c r="C28" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="25"/>
+      <c r="N28" s="25"/>
+      <c r="O28" s="25"/>
+      <c r="P28" s="25"/>
+    </row>
+    <row r="29" spans="1:16" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="31" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-    </row>
-    <row r="26" spans="1:4" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-    </row>
-    <row r="27" spans="1:4" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-    </row>
-    <row r="28" spans="1:4" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
+      <c r="C29" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="25"/>
+      <c r="N29" s="25"/>
+      <c r="O29" s="25"/>
+      <c r="P29" s="25"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" s="32"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="32"/>
+      <c r="O30" s="32"/>
+      <c r="P30" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>